<commit_message>
Long Term Portfolio Update
</commit_message>
<xml_diff>
--- a/portfolios/portfolio-2025-06-04.xlsx
+++ b/portfolios/portfolio-2025-06-04.xlsx
@@ -78822,10 +78822,10 @@
         <v>0.285</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.5145999999999999</v>
+        <v>0.4977</v>
       </c>
       <c r="BQ2" t="n">
-        <v>0.5671</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="BR2" t="n">
         <v>0.5</v>
@@ -79037,25 +79037,25 @@
         <v>190</v>
       </c>
       <c r="BK3" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="BL3" t="n">
-        <v>0.6137</v>
+        <v>0.605</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.0286</v>
+        <v>0.0556</v>
       </c>
       <c r="BN3" t="n">
-        <v>0.5714</v>
+        <v>0.5556</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.2275</v>
+        <v>0.21</v>
       </c>
       <c r="BP3" t="n">
-        <v>0.5145999999999999</v>
+        <v>0.4977</v>
       </c>
       <c r="BQ3" t="n">
-        <v>0.5671</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="BR3" t="n">
         <v>0.5</v>

</xml_diff>